<commit_message>
Update 15.05.2022 Realisierung startet
</commit_message>
<xml_diff>
--- a/Dokumentation/Zeitplan_joao_Correia.xlsx
+++ b/Dokumentation/Zeitplan_joao_Correia.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\00_project\ipa_joao\Dokumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\00_project\ipa_joao\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76F23E1-96D6-4335-8698-A810D50530CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA921053-BDC2-4C92-94F1-5DE645CFEB57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B89AD676-944C-450D-93C2-5644D63A8514}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{B89AD676-944C-450D-93C2-5644D63A8514}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <definedName name="_Toc103062712" localSheetId="0">Tabelle1!$A$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -339,9 +340,6 @@
     <t>5.2</t>
   </si>
   <si>
-    <t>5.3</t>
-  </si>
-  <si>
     <t>5.4</t>
   </si>
   <si>
@@ -505,6 +503,9 @@
   </si>
   <si>
     <t>Texturen Verzeichnis</t>
+  </si>
+  <si>
+    <t>8.3</t>
   </si>
 </sst>
 </file>
@@ -953,7 +954,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1117,6 +1118,25 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1135,28 +1155,9 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1473,8 +1474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E724F4-8276-4FB5-885D-8ADC5A3409FB}">
   <dimension ref="A1:AM89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P38" sqref="P38"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF64" sqref="AF64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1562,115 +1563,115 @@
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="33"/>
-      <c r="B9" s="99" t="s">
+      <c r="B9" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="100" t="s">
+      <c r="C9" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="97" t="s">
+      <c r="D9" s="103" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="98"/>
-      <c r="F9" s="98"/>
-      <c r="G9" s="98"/>
-      <c r="H9" s="98"/>
-      <c r="I9" s="98"/>
-      <c r="J9" s="98"/>
-      <c r="K9" s="98"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="98"/>
-      <c r="N9" s="98"/>
-      <c r="O9" s="98"/>
-      <c r="P9" s="98"/>
-      <c r="Q9" s="98"/>
-      <c r="R9" s="98"/>
-      <c r="S9" s="98"/>
-      <c r="T9" s="98"/>
-      <c r="U9" s="98"/>
-      <c r="V9" s="98"/>
-      <c r="W9" s="98"/>
-      <c r="X9" s="98"/>
-      <c r="Y9" s="98"/>
-      <c r="Z9" s="98"/>
-      <c r="AA9" s="98"/>
-      <c r="AB9" s="98"/>
-      <c r="AC9" s="98"/>
-      <c r="AD9" s="98"/>
-      <c r="AE9" s="98"/>
-      <c r="AF9" s="98"/>
-      <c r="AG9" s="98"/>
-      <c r="AH9" s="98"/>
-      <c r="AI9" s="98"/>
-      <c r="AJ9" s="98"/>
-      <c r="AK9" s="98"/>
-      <c r="AL9" s="98"/>
-      <c r="AM9" s="98"/>
+      <c r="E9" s="104"/>
+      <c r="F9" s="104"/>
+      <c r="G9" s="104"/>
+      <c r="H9" s="104"/>
+      <c r="I9" s="104"/>
+      <c r="J9" s="104"/>
+      <c r="K9" s="104"/>
+      <c r="L9" s="104"/>
+      <c r="M9" s="104"/>
+      <c r="N9" s="104"/>
+      <c r="O9" s="104"/>
+      <c r="P9" s="104"/>
+      <c r="Q9" s="104"/>
+      <c r="R9" s="104"/>
+      <c r="S9" s="104"/>
+      <c r="T9" s="104"/>
+      <c r="U9" s="104"/>
+      <c r="V9" s="104"/>
+      <c r="W9" s="104"/>
+      <c r="X9" s="104"/>
+      <c r="Y9" s="104"/>
+      <c r="Z9" s="104"/>
+      <c r="AA9" s="104"/>
+      <c r="AB9" s="104"/>
+      <c r="AC9" s="104"/>
+      <c r="AD9" s="104"/>
+      <c r="AE9" s="104"/>
+      <c r="AF9" s="104"/>
+      <c r="AG9" s="104"/>
+      <c r="AH9" s="104"/>
+      <c r="AI9" s="104"/>
+      <c r="AJ9" s="104"/>
+      <c r="AK9" s="104"/>
+      <c r="AL9" s="104"/>
+      <c r="AM9" s="104"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
-      <c r="B10" s="99"/>
-      <c r="C10" s="100"/>
-      <c r="D10" s="101" t="s">
+      <c r="B10" s="94"/>
+      <c r="C10" s="95"/>
+      <c r="D10" s="96" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" s="97"/>
+      <c r="F10" s="98"/>
+      <c r="G10" s="99" t="s">
         <v>113</v>
       </c>
-      <c r="E10" s="102"/>
-      <c r="F10" s="103"/>
-      <c r="G10" s="93" t="s">
+      <c r="H10" s="100"/>
+      <c r="I10" s="101"/>
+      <c r="J10" s="99" t="s">
         <v>114</v>
       </c>
-      <c r="H10" s="94"/>
-      <c r="I10" s="95"/>
-      <c r="J10" s="93" t="s">
+      <c r="K10" s="100"/>
+      <c r="L10" s="101"/>
+      <c r="M10" s="99" t="s">
         <v>115</v>
       </c>
-      <c r="K10" s="94"/>
-      <c r="L10" s="95"/>
-      <c r="M10" s="93" t="s">
+      <c r="N10" s="100"/>
+      <c r="O10" s="101"/>
+      <c r="P10" s="99" t="s">
         <v>116</v>
       </c>
-      <c r="N10" s="94"/>
-      <c r="O10" s="95"/>
-      <c r="P10" s="93" t="s">
+      <c r="Q10" s="100"/>
+      <c r="R10" s="101"/>
+      <c r="S10" s="99" t="s">
         <v>117</v>
       </c>
-      <c r="Q10" s="94"/>
-      <c r="R10" s="95"/>
-      <c r="S10" s="93" t="s">
+      <c r="T10" s="100"/>
+      <c r="U10" s="101"/>
+      <c r="V10" s="99" t="s">
         <v>118</v>
       </c>
-      <c r="T10" s="94"/>
-      <c r="U10" s="95"/>
-      <c r="V10" s="93" t="s">
+      <c r="W10" s="100"/>
+      <c r="X10" s="101"/>
+      <c r="Y10" s="99" t="s">
         <v>119</v>
       </c>
-      <c r="W10" s="94"/>
-      <c r="X10" s="95"/>
-      <c r="Y10" s="93" t="s">
+      <c r="Z10" s="100"/>
+      <c r="AA10" s="101"/>
+      <c r="AB10" s="99" t="s">
         <v>120</v>
       </c>
-      <c r="Z10" s="94"/>
-      <c r="AA10" s="95"/>
-      <c r="AB10" s="93" t="s">
+      <c r="AC10" s="100"/>
+      <c r="AD10" s="101"/>
+      <c r="AE10" s="99" t="s">
         <v>121</v>
       </c>
-      <c r="AC10" s="94"/>
-      <c r="AD10" s="95"/>
-      <c r="AE10" s="93" t="s">
+      <c r="AF10" s="100"/>
+      <c r="AG10" s="102"/>
+      <c r="AH10" s="99" t="s">
         <v>122</v>
       </c>
-      <c r="AF10" s="94"/>
-      <c r="AG10" s="96"/>
-      <c r="AH10" s="93" t="s">
+      <c r="AI10" s="100"/>
+      <c r="AJ10" s="102"/>
+      <c r="AK10" s="99" t="s">
         <v>123</v>
       </c>
-      <c r="AI10" s="94"/>
-      <c r="AJ10" s="96"/>
-      <c r="AK10" s="93" t="s">
-        <v>124</v>
-      </c>
-      <c r="AL10" s="94"/>
-      <c r="AM10" s="96"/>
+      <c r="AL10" s="100"/>
+      <c r="AM10" s="102"/>
     </row>
     <row r="11" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="35"/>
@@ -2407,10 +2408,10 @@
     <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C24" s="76" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
@@ -2455,10 +2456,10 @@
     <row r="25" spans="1:39" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="58" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" s="78" t="s">
         <v>125</v>
-      </c>
-      <c r="C25" s="78" t="s">
-        <v>126</v>
       </c>
       <c r="D25" s="54"/>
       <c r="E25" s="54"/>
@@ -2597,7 +2598,7 @@
         <v>64</v>
       </c>
       <c r="C28" s="76" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D28" s="25"/>
       <c r="E28" s="25"/>
@@ -2838,7 +2839,7 @@
         <v>27</v>
       </c>
       <c r="C33" s="77" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D33" s="25"/>
       <c r="E33" s="25"/>
@@ -2887,7 +2888,7 @@
         <v>28</v>
       </c>
       <c r="C34" s="76" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="25"/>
@@ -2977,11 +2978,11 @@
     </row>
     <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="31" t="s">
         <v>30</v>
       </c>
       <c r="C36" s="76" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D36" s="25"/>
       <c r="E36" s="25"/>
@@ -2998,11 +2999,19 @@
       <c r="P36" s="25">
         <v>2</v>
       </c>
-      <c r="Q36" s="26"/>
-      <c r="R36" s="27"/>
-      <c r="S36" s="25"/>
+      <c r="Q36" s="92">
+        <v>1</v>
+      </c>
+      <c r="R36" s="52">
+        <v>1</v>
+      </c>
+      <c r="S36" s="25">
+        <v>1</v>
+      </c>
       <c r="T36" s="26"/>
-      <c r="U36" s="27"/>
+      <c r="U36" s="52">
+        <v>1</v>
+      </c>
       <c r="V36" s="25"/>
       <c r="W36" s="26"/>
       <c r="X36" s="27"/>
@@ -3028,7 +3037,7 @@
         <v>99</v>
       </c>
       <c r="C37" s="76" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D37" s="25"/>
       <c r="E37" s="25"/>
@@ -3072,11 +3081,11 @@
     </row>
     <row r="38" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
-      <c r="B38" s="104" t="s">
+      <c r="B38" s="31" t="s">
         <v>100</v>
       </c>
       <c r="C38" s="76" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D38" s="25"/>
       <c r="E38" s="25"/>
@@ -3087,13 +3096,15 @@
       <c r="J38" s="25"/>
       <c r="K38" s="26"/>
       <c r="L38" s="27"/>
-      <c r="M38" s="105"/>
-      <c r="N38" s="68"/>
+      <c r="M38" s="25"/>
+      <c r="N38" s="26"/>
       <c r="O38" s="27"/>
-      <c r="P38">
-        <v>1</v>
-      </c>
-      <c r="Q38" s="26"/>
+      <c r="P38" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="Q38" s="92">
+        <v>0.2</v>
+      </c>
       <c r="R38" s="27"/>
       <c r="S38" s="25"/>
       <c r="T38" s="26"/>
@@ -3118,7 +3129,6 @@
       <c r="AM38" s="27"/>
     </row>
     <row r="39" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
       <c r="B39" s="31" t="s">
         <v>101</v>
       </c>
@@ -3138,10 +3148,10 @@
       <c r="N39" s="26"/>
       <c r="O39" s="27"/>
       <c r="P39" s="25">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q39" s="92">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="R39" s="27"/>
       <c r="S39" s="25"/>
@@ -3167,11 +3177,12 @@
       <c r="AM39" s="27"/>
     </row>
     <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
       <c r="B40" s="31" t="s">
         <v>102</v>
       </c>
       <c r="C40" s="76" t="s">
-        <v>150</v>
+        <v>72</v>
       </c>
       <c r="D40" s="25"/>
       <c r="E40" s="25"/>
@@ -3188,13 +3199,17 @@
       <c r="P40" s="25">
         <v>1</v>
       </c>
-      <c r="Q40" s="92">
-        <v>0.1</v>
-      </c>
-      <c r="R40" s="27"/>
-      <c r="S40" s="25"/>
+      <c r="Q40" s="26"/>
+      <c r="R40" s="52">
+        <v>1</v>
+      </c>
+      <c r="S40" s="25">
+        <v>0.5</v>
+      </c>
       <c r="T40" s="26"/>
-      <c r="U40" s="27"/>
+      <c r="U40" s="27">
+        <v>0.5</v>
+      </c>
       <c r="V40" s="25"/>
       <c r="W40" s="26"/>
       <c r="X40" s="27"/>
@@ -3214,150 +3229,150 @@
       <c r="AL40" s="26"/>
       <c r="AM40" s="27"/>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="104" t="s">
+    <row r="41" spans="1:39" s="56" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
+      <c r="B41" s="58" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" s="78" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41" s="54"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="55"/>
+      <c r="G41" s="54"/>
+      <c r="H41" s="53"/>
+      <c r="I41" s="55"/>
+      <c r="J41" s="54"/>
+      <c r="K41" s="53"/>
+      <c r="L41" s="55"/>
+      <c r="M41" s="54"/>
+      <c r="N41" s="53"/>
+      <c r="O41" s="55"/>
+      <c r="P41" s="54"/>
+      <c r="Q41" s="53"/>
+      <c r="R41" s="55"/>
+      <c r="S41" s="54"/>
+      <c r="T41" s="53"/>
+      <c r="U41" s="55"/>
+      <c r="V41" s="54"/>
+      <c r="W41" s="53"/>
+      <c r="X41" s="55"/>
+      <c r="Y41" s="54"/>
+      <c r="Z41" s="53"/>
+      <c r="AA41" s="55"/>
+      <c r="AB41" s="54"/>
+      <c r="AC41" s="53"/>
+      <c r="AD41" s="55"/>
+      <c r="AE41" s="54"/>
+      <c r="AF41" s="53"/>
+      <c r="AG41" s="55"/>
+      <c r="AH41" s="54"/>
+      <c r="AI41" s="53"/>
+      <c r="AJ41" s="55"/>
+      <c r="AK41" s="54"/>
+      <c r="AL41" s="53"/>
+      <c r="AM41" s="55"/>
+    </row>
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
+      <c r="B42" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="C41" s="76" t="s">
-        <v>72</v>
-      </c>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="26"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="26"/>
-      <c r="L41" s="27"/>
-      <c r="M41" s="25"/>
-      <c r="N41" s="26"/>
-      <c r="O41" s="27"/>
-      <c r="P41" s="25">
-        <v>1</v>
-      </c>
-      <c r="Q41" s="26"/>
-      <c r="R41" s="27"/>
-      <c r="S41" s="25"/>
-      <c r="T41" s="26"/>
-      <c r="U41" s="27"/>
-      <c r="V41" s="25"/>
-      <c r="W41" s="26"/>
-      <c r="X41" s="27"/>
-      <c r="Y41" s="25"/>
-      <c r="Z41" s="26"/>
-      <c r="AA41" s="27"/>
-      <c r="AB41" s="25"/>
-      <c r="AC41" s="26"/>
-      <c r="AD41" s="27"/>
-      <c r="AE41" s="25"/>
-      <c r="AF41" s="26"/>
-      <c r="AG41" s="27"/>
-      <c r="AH41" s="25"/>
-      <c r="AI41" s="26"/>
-      <c r="AJ41" s="27"/>
-      <c r="AK41" s="25"/>
-      <c r="AL41" s="26"/>
-      <c r="AM41" s="27"/>
-    </row>
-    <row r="42" spans="1:39" s="56" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
-      <c r="B42" s="58" t="s">
-        <v>125</v>
-      </c>
-      <c r="C42" s="78" t="s">
-        <v>127</v>
-      </c>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54"/>
-      <c r="F42" s="55"/>
-      <c r="G42" s="54"/>
-      <c r="H42" s="53"/>
-      <c r="I42" s="55"/>
-      <c r="J42" s="54"/>
-      <c r="K42" s="53"/>
-      <c r="L42" s="55"/>
-      <c r="M42" s="54"/>
-      <c r="N42" s="53"/>
-      <c r="O42" s="55"/>
-      <c r="P42" s="54"/>
-      <c r="Q42" s="53"/>
-      <c r="R42" s="55"/>
-      <c r="S42" s="54"/>
-      <c r="T42" s="53"/>
-      <c r="U42" s="55"/>
-      <c r="V42" s="54"/>
-      <c r="W42" s="53"/>
-      <c r="X42" s="55"/>
-      <c r="Y42" s="54"/>
-      <c r="Z42" s="53"/>
-      <c r="AA42" s="55"/>
-      <c r="AB42" s="54"/>
-      <c r="AC42" s="53"/>
-      <c r="AD42" s="55"/>
-      <c r="AE42" s="54"/>
-      <c r="AF42" s="53"/>
-      <c r="AG42" s="55"/>
-      <c r="AH42" s="54"/>
-      <c r="AI42" s="53"/>
-      <c r="AJ42" s="55"/>
-      <c r="AK42" s="54"/>
-      <c r="AL42" s="53"/>
-      <c r="AM42" s="55"/>
+      <c r="C42" s="79" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="47"/>
+      <c r="J42" s="28"/>
+      <c r="K42" s="28"/>
+      <c r="L42" s="47"/>
+      <c r="M42" s="28"/>
+      <c r="N42" s="28"/>
+      <c r="O42" s="47"/>
+      <c r="P42" s="28"/>
+      <c r="Q42" s="28"/>
+      <c r="R42" s="47"/>
+      <c r="S42" s="28"/>
+      <c r="T42" s="28"/>
+      <c r="U42" s="47"/>
+      <c r="V42" s="28"/>
+      <c r="W42" s="28"/>
+      <c r="X42" s="47"/>
+      <c r="Y42" s="28"/>
+      <c r="Z42" s="28"/>
+      <c r="AA42" s="47"/>
+      <c r="AB42" s="28"/>
+      <c r="AC42" s="28"/>
+      <c r="AD42" s="47"/>
+      <c r="AE42" s="28"/>
+      <c r="AF42" s="28"/>
+      <c r="AG42" s="47"/>
+      <c r="AH42" s="28"/>
+      <c r="AI42" s="28"/>
+      <c r="AJ42" s="47"/>
+      <c r="AK42" s="28"/>
+      <c r="AL42" s="28"/>
+      <c r="AM42" s="47"/>
     </row>
     <row r="43" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
-      <c r="B43" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="C43" s="79" t="s">
-        <v>26</v>
-      </c>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
-      <c r="H43" s="28"/>
-      <c r="I43" s="47"/>
-      <c r="J43" s="28"/>
-      <c r="K43" s="28"/>
-      <c r="L43" s="47"/>
-      <c r="M43" s="28"/>
-      <c r="N43" s="28"/>
-      <c r="O43" s="47"/>
-      <c r="P43" s="28"/>
-      <c r="Q43" s="28"/>
-      <c r="R43" s="47"/>
-      <c r="S43" s="28"/>
-      <c r="T43" s="28"/>
-      <c r="U43" s="47"/>
-      <c r="V43" s="28"/>
-      <c r="W43" s="28"/>
-      <c r="X43" s="47"/>
-      <c r="Y43" s="28"/>
-      <c r="Z43" s="28"/>
-      <c r="AA43" s="47"/>
-      <c r="AB43" s="28"/>
-      <c r="AC43" s="28"/>
-      <c r="AD43" s="47"/>
-      <c r="AE43" s="28"/>
-      <c r="AF43" s="28"/>
-      <c r="AG43" s="47"/>
-      <c r="AH43" s="28"/>
-      <c r="AI43" s="28"/>
-      <c r="AJ43" s="47"/>
-      <c r="AK43" s="28"/>
-      <c r="AL43" s="28"/>
-      <c r="AM43" s="47"/>
+      <c r="B43" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="77" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="26"/>
+      <c r="L43" s="27"/>
+      <c r="M43" s="25"/>
+      <c r="N43" s="26"/>
+      <c r="O43" s="27"/>
+      <c r="P43" s="25"/>
+      <c r="Q43" s="26"/>
+      <c r="R43" s="105"/>
+      <c r="S43" s="106"/>
+      <c r="T43" s="26"/>
+      <c r="U43" s="27"/>
+      <c r="V43" s="25">
+        <v>1</v>
+      </c>
+      <c r="W43" s="26"/>
+      <c r="X43" s="105"/>
+      <c r="Y43" s="106"/>
+      <c r="Z43" s="26"/>
+      <c r="AA43" s="27"/>
+      <c r="AB43" s="25"/>
+      <c r="AC43" s="26"/>
+      <c r="AD43" s="27"/>
+      <c r="AE43" s="25"/>
+      <c r="AF43" s="26"/>
+      <c r="AG43" s="27"/>
+      <c r="AH43" s="25"/>
+      <c r="AI43" s="26"/>
+      <c r="AJ43" s="27"/>
+      <c r="AK43" s="25"/>
+      <c r="AL43" s="26"/>
+      <c r="AM43" s="27"/>
     </row>
     <row r="44" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="29" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C44" s="77" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D44" s="25"/>
       <c r="E44" s="25"/>
@@ -3373,16 +3388,16 @@
       <c r="O44" s="27"/>
       <c r="P44" s="25"/>
       <c r="Q44" s="26"/>
-      <c r="R44" s="27"/>
-      <c r="S44" s="25">
-        <v>1</v>
-      </c>
+      <c r="R44" s="105"/>
+      <c r="S44" s="106"/>
       <c r="T44" s="26"/>
       <c r="U44" s="27"/>
-      <c r="V44" s="25"/>
+      <c r="V44" s="25">
+        <v>0.5</v>
+      </c>
       <c r="W44" s="26"/>
-      <c r="X44" s="27"/>
-      <c r="Y44" s="25"/>
+      <c r="X44" s="105"/>
+      <c r="Y44" s="106"/>
       <c r="Z44" s="26"/>
       <c r="AA44" s="27"/>
       <c r="AB44" s="25"/>
@@ -3401,10 +3416,10 @@
     <row r="45" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C45" s="77" t="s">
-        <v>78</v>
+        <v>35</v>
+      </c>
+      <c r="C45" s="81" t="s">
+        <v>74</v>
       </c>
       <c r="D45" s="25"/>
       <c r="E45" s="25"/>
@@ -3420,16 +3435,16 @@
       <c r="O45" s="27"/>
       <c r="P45" s="25"/>
       <c r="Q45" s="26"/>
-      <c r="R45" s="27"/>
-      <c r="S45" s="25">
-        <v>0.5</v>
-      </c>
+      <c r="R45" s="105"/>
+      <c r="S45" s="106"/>
       <c r="T45" s="26"/>
       <c r="U45" s="27"/>
-      <c r="V45" s="25"/>
+      <c r="V45" s="25">
+        <v>1</v>
+      </c>
       <c r="W45" s="26"/>
-      <c r="X45" s="27"/>
-      <c r="Y45" s="25"/>
+      <c r="X45" s="105"/>
+      <c r="Y45" s="106"/>
       <c r="Z45" s="26"/>
       <c r="AA45" s="27"/>
       <c r="AB45" s="25"/>
@@ -3448,10 +3463,10 @@
     <row r="46" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C46" s="81" t="s">
-        <v>74</v>
+        <v>36</v>
+      </c>
+      <c r="C46" s="77" t="s">
+        <v>75</v>
       </c>
       <c r="D46" s="25"/>
       <c r="E46" s="25"/>
@@ -3467,16 +3482,16 @@
       <c r="O46" s="27"/>
       <c r="P46" s="25"/>
       <c r="Q46" s="26"/>
-      <c r="R46" s="27"/>
-      <c r="S46" s="25">
-        <v>1</v>
-      </c>
+      <c r="R46" s="105"/>
+      <c r="S46" s="106"/>
       <c r="T46" s="26"/>
       <c r="U46" s="27"/>
-      <c r="V46" s="25"/>
+      <c r="V46" s="25">
+        <v>2</v>
+      </c>
       <c r="W46" s="26"/>
-      <c r="X46" s="27"/>
-      <c r="Y46" s="25"/>
+      <c r="X46" s="105"/>
+      <c r="Y46" s="106"/>
       <c r="Z46" s="26"/>
       <c r="AA46" s="27"/>
       <c r="AB46" s="25"/>
@@ -3495,10 +3510,10 @@
     <row r="47" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="29" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C47" s="77" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D47" s="25"/>
       <c r="E47" s="25"/>
@@ -3514,16 +3529,16 @@
       <c r="O47" s="27"/>
       <c r="P47" s="25"/>
       <c r="Q47" s="26"/>
-      <c r="R47" s="27"/>
-      <c r="S47" s="25">
-        <v>2</v>
-      </c>
+      <c r="R47" s="105"/>
+      <c r="S47" s="106"/>
       <c r="T47" s="26"/>
-      <c r="U47" s="27"/>
-      <c r="V47" s="25"/>
+      <c r="U47" s="105"/>
+      <c r="V47" s="26"/>
       <c r="W47" s="26"/>
       <c r="X47" s="27"/>
-      <c r="Y47" s="25"/>
+      <c r="Y47" s="25">
+        <v>1</v>
+      </c>
       <c r="Z47" s="26"/>
       <c r="AA47" s="27"/>
       <c r="AB47" s="25"/>
@@ -3542,10 +3557,10 @@
     <row r="48" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="29" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C48" s="77" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D48" s="25"/>
       <c r="E48" s="25"/>
@@ -3562,15 +3577,15 @@
       <c r="P48" s="25"/>
       <c r="Q48" s="26"/>
       <c r="R48" s="27"/>
-      <c r="S48" s="25">
-        <v>1</v>
-      </c>
+      <c r="S48" s="25"/>
       <c r="T48" s="26"/>
-      <c r="U48" s="27"/>
-      <c r="V48" s="25"/>
+      <c r="U48" s="105"/>
+      <c r="V48" s="106"/>
       <c r="W48" s="26"/>
       <c r="X48" s="27"/>
-      <c r="Y48" s="25"/>
+      <c r="Y48" s="25">
+        <v>1</v>
+      </c>
       <c r="Z48" s="26"/>
       <c r="AA48" s="27"/>
       <c r="AB48" s="25"/>
@@ -3589,10 +3604,10 @@
     <row r="49" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="C49" s="77" t="s">
-        <v>77</v>
+        <v>39</v>
+      </c>
+      <c r="C49" s="81" t="s">
+        <v>80</v>
       </c>
       <c r="D49" s="25"/>
       <c r="E49" s="25"/>
@@ -3611,13 +3626,13 @@
       <c r="R49" s="27"/>
       <c r="S49" s="25"/>
       <c r="T49" s="26"/>
-      <c r="U49" s="27"/>
-      <c r="V49" s="25">
-        <v>1</v>
-      </c>
+      <c r="U49" s="105"/>
+      <c r="V49" s="106"/>
       <c r="W49" s="26"/>
       <c r="X49" s="27"/>
-      <c r="Y49" s="25"/>
+      <c r="Y49" s="25">
+        <v>2</v>
+      </c>
       <c r="Z49" s="26"/>
       <c r="AA49" s="27"/>
       <c r="AB49" s="25"/>
@@ -3633,13 +3648,13 @@
       <c r="AL49" s="26"/>
       <c r="AM49" s="27"/>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:39" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C50" s="81" t="s">
-        <v>80</v>
+        <v>105</v>
+      </c>
+      <c r="C50" s="77" t="s">
+        <v>81</v>
       </c>
       <c r="D50" s="25"/>
       <c r="E50" s="25"/>
@@ -3658,13 +3673,13 @@
       <c r="R50" s="27"/>
       <c r="S50" s="25"/>
       <c r="T50" s="26"/>
-      <c r="U50" s="27"/>
-      <c r="V50" s="25">
-        <v>2</v>
-      </c>
+      <c r="U50" s="105"/>
+      <c r="V50" s="106"/>
       <c r="W50" s="26"/>
       <c r="X50" s="27"/>
-      <c r="Y50" s="25"/>
+      <c r="Y50" s="25">
+        <v>0.5</v>
+      </c>
       <c r="Z50" s="26"/>
       <c r="AA50" s="27"/>
       <c r="AB50" s="25"/>
@@ -3680,97 +3695,97 @@
       <c r="AL50" s="26"/>
       <c r="AM50" s="27"/>
     </row>
-    <row r="51" spans="1:39" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:39" s="46" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
-      <c r="B51" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="C51" s="77" t="s">
-        <v>81</v>
-      </c>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
-      <c r="F51" s="27"/>
-      <c r="G51" s="25"/>
-      <c r="H51" s="26"/>
-      <c r="I51" s="27"/>
-      <c r="J51" s="25"/>
-      <c r="K51" s="26"/>
-      <c r="L51" s="27"/>
-      <c r="M51" s="25"/>
-      <c r="N51" s="26"/>
-      <c r="O51" s="27"/>
-      <c r="P51" s="25"/>
-      <c r="Q51" s="26"/>
-      <c r="R51" s="27"/>
-      <c r="S51" s="25"/>
-      <c r="T51" s="26"/>
-      <c r="U51" s="27"/>
-      <c r="V51" s="25">
-        <v>0.5</v>
-      </c>
-      <c r="W51" s="26"/>
-      <c r="X51" s="27"/>
-      <c r="Y51" s="25"/>
-      <c r="Z51" s="26"/>
-      <c r="AA51" s="27"/>
-      <c r="AB51" s="25"/>
-      <c r="AC51" s="26"/>
-      <c r="AD51" s="27"/>
-      <c r="AE51" s="25"/>
-      <c r="AF51" s="26"/>
-      <c r="AG51" s="27"/>
-      <c r="AH51" s="25"/>
-      <c r="AI51" s="26"/>
-      <c r="AJ51" s="27"/>
-      <c r="AK51" s="25"/>
-      <c r="AL51" s="26"/>
-      <c r="AM51" s="27"/>
-    </row>
-    <row r="52" spans="1:39" s="46" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="C51" s="91" t="s">
+        <v>79</v>
+      </c>
+      <c r="D51" s="44"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="45"/>
+      <c r="G51" s="44"/>
+      <c r="H51" s="43"/>
+      <c r="I51" s="45"/>
+      <c r="J51" s="44"/>
+      <c r="K51" s="43"/>
+      <c r="L51" s="45"/>
+      <c r="M51" s="44"/>
+      <c r="N51" s="43"/>
+      <c r="O51" s="45"/>
+      <c r="P51" s="44"/>
+      <c r="Q51" s="43"/>
+      <c r="R51" s="45"/>
+      <c r="S51" s="44"/>
+      <c r="T51" s="43"/>
+      <c r="U51" s="107"/>
+      <c r="V51" s="43"/>
+      <c r="W51" s="43"/>
+      <c r="X51" s="45"/>
+      <c r="Y51" s="44"/>
+      <c r="Z51" s="43"/>
+      <c r="AA51" s="45"/>
+      <c r="AB51" s="44"/>
+      <c r="AC51" s="43"/>
+      <c r="AD51" s="45"/>
+      <c r="AE51" s="44"/>
+      <c r="AF51" s="43"/>
+      <c r="AG51" s="45"/>
+      <c r="AH51" s="44"/>
+      <c r="AI51" s="43"/>
+      <c r="AJ51" s="45"/>
+      <c r="AK51" s="44"/>
+      <c r="AL51" s="43"/>
+      <c r="AM51" s="45"/>
+    </row>
+    <row r="52" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
-      <c r="B52" s="42" t="s">
+      <c r="B52" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="C52" s="91" t="s">
-        <v>79</v>
-      </c>
-      <c r="D52" s="44"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="45"/>
-      <c r="G52" s="44"/>
-      <c r="H52" s="43"/>
-      <c r="I52" s="45"/>
-      <c r="J52" s="44"/>
-      <c r="K52" s="43"/>
-      <c r="L52" s="45"/>
-      <c r="M52" s="44"/>
-      <c r="N52" s="43"/>
-      <c r="O52" s="45"/>
-      <c r="P52" s="44"/>
-      <c r="Q52" s="43"/>
-      <c r="R52" s="45"/>
-      <c r="S52" s="44"/>
-      <c r="T52" s="43"/>
-      <c r="U52" s="45"/>
-      <c r="V52" s="44"/>
-      <c r="W52" s="43"/>
-      <c r="X52" s="45"/>
-      <c r="Y52" s="44"/>
-      <c r="Z52" s="43"/>
-      <c r="AA52" s="45"/>
-      <c r="AB52" s="44"/>
-      <c r="AC52" s="43"/>
-      <c r="AD52" s="45"/>
-      <c r="AE52" s="44"/>
-      <c r="AF52" s="43"/>
-      <c r="AG52" s="45"/>
-      <c r="AH52" s="44"/>
-      <c r="AI52" s="43"/>
-      <c r="AJ52" s="45"/>
-      <c r="AK52" s="44"/>
-      <c r="AL52" s="43"/>
-      <c r="AM52" s="45"/>
+      <c r="C52" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="D52" s="25"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="27"/>
+      <c r="G52" s="25"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="27"/>
+      <c r="J52" s="25"/>
+      <c r="K52" s="26"/>
+      <c r="L52" s="27"/>
+      <c r="M52" s="25"/>
+      <c r="N52" s="26"/>
+      <c r="O52" s="27"/>
+      <c r="P52" s="25"/>
+      <c r="Q52" s="26"/>
+      <c r="R52" s="27"/>
+      <c r="S52" s="25"/>
+      <c r="T52" s="26"/>
+      <c r="U52" s="105"/>
+      <c r="V52" s="106"/>
+      <c r="W52" s="26"/>
+      <c r="X52" s="27"/>
+      <c r="Y52" s="25">
+        <v>2</v>
+      </c>
+      <c r="Z52" s="26"/>
+      <c r="AA52" s="27"/>
+      <c r="AB52" s="25"/>
+      <c r="AC52" s="26"/>
+      <c r="AD52" s="27"/>
+      <c r="AE52" s="25"/>
+      <c r="AF52" s="26"/>
+      <c r="AG52" s="27"/>
+      <c r="AH52" s="25"/>
+      <c r="AI52" s="26"/>
+      <c r="AJ52" s="27"/>
+      <c r="AK52" s="25"/>
+      <c r="AL52" s="26"/>
+      <c r="AM52" s="27"/>
     </row>
     <row r="53" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
@@ -3778,7 +3793,7 @@
         <v>110</v>
       </c>
       <c r="C53" s="77" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D53" s="25"/>
       <c r="E53" s="25"/>
@@ -3797,13 +3812,13 @@
       <c r="R53" s="27"/>
       <c r="S53" s="25"/>
       <c r="T53" s="26"/>
-      <c r="U53" s="27"/>
-      <c r="V53" s="25">
-        <v>2</v>
-      </c>
+      <c r="U53" s="105"/>
+      <c r="V53" s="106"/>
       <c r="W53" s="26"/>
       <c r="X53" s="27"/>
-      <c r="Y53" s="25"/>
+      <c r="Y53" s="25">
+        <v>1.5</v>
+      </c>
       <c r="Z53" s="26"/>
       <c r="AA53" s="27"/>
       <c r="AB53" s="25"/>
@@ -3825,7 +3840,7 @@
         <v>111</v>
       </c>
       <c r="C54" s="77" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D54" s="25"/>
       <c r="E54" s="25"/>
@@ -3844,14 +3859,12 @@
       <c r="R54" s="27"/>
       <c r="S54" s="25"/>
       <c r="T54" s="26"/>
-      <c r="U54" s="27"/>
-      <c r="V54" s="25">
-        <v>0.5</v>
-      </c>
+      <c r="U54" s="105"/>
+      <c r="V54" s="26"/>
       <c r="W54" s="26"/>
       <c r="X54" s="27"/>
       <c r="Y54" s="25">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Z54" s="26"/>
       <c r="AA54" s="27"/>
@@ -3869,12 +3882,11 @@
       <c r="AM54" s="27"/>
     </row>
     <row r="55" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A55" s="8"/>
       <c r="B55" s="29" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="C55" s="77" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D55" s="25"/>
       <c r="E55" s="25"/>
@@ -3893,12 +3905,12 @@
       <c r="R55" s="27"/>
       <c r="S55" s="25"/>
       <c r="T55" s="26"/>
-      <c r="U55" s="27"/>
-      <c r="V55" s="25"/>
+      <c r="U55" s="105"/>
+      <c r="V55" s="26"/>
       <c r="W55" s="26"/>
       <c r="X55" s="27"/>
       <c r="Y55" s="25">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="Z55" s="26"/>
       <c r="AA55" s="27"/>
@@ -3915,104 +3927,104 @@
       <c r="AL55" s="26"/>
       <c r="AM55" s="27"/>
     </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="B56" s="29" t="s">
+    <row r="56" spans="1:39" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56"/>
+      <c r="B56" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="C56" s="91" t="s">
         <v>138</v>
       </c>
-      <c r="C56" s="77" t="s">
-        <v>86</v>
-      </c>
-      <c r="D56" s="25"/>
-      <c r="E56" s="25"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="25"/>
-      <c r="H56" s="26"/>
-      <c r="I56" s="27"/>
-      <c r="J56" s="25"/>
-      <c r="K56" s="26"/>
-      <c r="L56" s="27"/>
-      <c r="M56" s="25"/>
-      <c r="N56" s="26"/>
-      <c r="O56" s="27"/>
-      <c r="P56" s="25"/>
-      <c r="Q56" s="26"/>
-      <c r="R56" s="27"/>
-      <c r="S56" s="25"/>
-      <c r="T56" s="26"/>
-      <c r="U56" s="27"/>
-      <c r="V56" s="25"/>
-      <c r="W56" s="26"/>
-      <c r="X56" s="27"/>
-      <c r="Y56" s="25">
-        <v>2</v>
-      </c>
-      <c r="Z56" s="26"/>
-      <c r="AA56" s="27"/>
-      <c r="AB56" s="25"/>
-      <c r="AC56" s="26"/>
-      <c r="AD56" s="27"/>
-      <c r="AE56" s="25"/>
-      <c r="AF56" s="26"/>
-      <c r="AG56" s="27"/>
-      <c r="AH56" s="25"/>
-      <c r="AI56" s="26"/>
-      <c r="AJ56" s="27"/>
-      <c r="AK56" s="25"/>
-      <c r="AL56" s="26"/>
-      <c r="AM56" s="27"/>
-    </row>
-    <row r="57" spans="1:39" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57"/>
-      <c r="B57" s="42" t="s">
-        <v>128</v>
-      </c>
-      <c r="C57" s="91" t="s">
-        <v>139</v>
-      </c>
-      <c r="D57" s="44"/>
-      <c r="E57" s="44"/>
-      <c r="F57" s="45"/>
-      <c r="G57" s="44"/>
-      <c r="H57" s="43"/>
-      <c r="I57" s="45"/>
-      <c r="J57" s="44"/>
-      <c r="K57" s="43"/>
-      <c r="L57" s="45"/>
-      <c r="M57" s="44"/>
-      <c r="N57" s="43"/>
-      <c r="O57" s="45"/>
-      <c r="P57" s="44"/>
-      <c r="Q57" s="43"/>
-      <c r="R57" s="45"/>
-      <c r="S57" s="44"/>
-      <c r="T57" s="43"/>
-      <c r="U57" s="45"/>
-      <c r="V57" s="44"/>
-      <c r="W57" s="43"/>
-      <c r="X57" s="45"/>
-      <c r="Y57" s="44"/>
-      <c r="Z57" s="43"/>
-      <c r="AA57" s="45"/>
-      <c r="AB57" s="44"/>
-      <c r="AC57" s="43"/>
-      <c r="AD57" s="45"/>
-      <c r="AE57" s="44"/>
-      <c r="AF57" s="43"/>
-      <c r="AG57" s="45"/>
-      <c r="AH57" s="44"/>
-      <c r="AI57" s="43"/>
-      <c r="AJ57" s="45"/>
-      <c r="AK57" s="44"/>
-      <c r="AL57" s="43"/>
-      <c r="AM57" s="45"/>
+      <c r="D56" s="44"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="45"/>
+      <c r="G56" s="44"/>
+      <c r="H56" s="43"/>
+      <c r="I56" s="45"/>
+      <c r="J56" s="44"/>
+      <c r="K56" s="43"/>
+      <c r="L56" s="45"/>
+      <c r="M56" s="44"/>
+      <c r="N56" s="43"/>
+      <c r="O56" s="45"/>
+      <c r="P56" s="44"/>
+      <c r="Q56" s="43"/>
+      <c r="R56" s="45"/>
+      <c r="S56" s="44"/>
+      <c r="T56" s="43"/>
+      <c r="U56" s="107"/>
+      <c r="V56" s="43"/>
+      <c r="W56" s="43"/>
+      <c r="X56" s="45"/>
+      <c r="Y56" s="44"/>
+      <c r="Z56" s="43"/>
+      <c r="AA56" s="45"/>
+      <c r="AB56" s="44"/>
+      <c r="AC56" s="43"/>
+      <c r="AD56" s="45"/>
+      <c r="AE56" s="44"/>
+      <c r="AF56" s="43"/>
+      <c r="AG56" s="45"/>
+      <c r="AH56" s="44"/>
+      <c r="AI56" s="43"/>
+      <c r="AJ56" s="45"/>
+      <c r="AK56" s="44"/>
+      <c r="AL56" s="43"/>
+      <c r="AM56" s="45"/>
+    </row>
+    <row r="57" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A57" s="8"/>
+      <c r="B57" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="C57" s="76" t="s">
+        <v>154</v>
+      </c>
+      <c r="D57" s="25"/>
+      <c r="E57" s="25"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="25"/>
+      <c r="H57" s="26"/>
+      <c r="I57" s="27"/>
+      <c r="J57" s="25"/>
+      <c r="K57" s="26"/>
+      <c r="L57" s="27"/>
+      <c r="M57" s="93"/>
+      <c r="N57" s="68"/>
+      <c r="O57" s="27"/>
+      <c r="Q57" s="26"/>
+      <c r="R57" s="27"/>
+      <c r="S57" s="25"/>
+      <c r="T57" s="26"/>
+      <c r="U57" s="27"/>
+      <c r="V57" s="25"/>
+      <c r="W57" s="26"/>
+      <c r="X57" s="27"/>
+      <c r="Y57" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="Z57" s="26"/>
+      <c r="AA57" s="27"/>
+      <c r="AB57" s="25"/>
+      <c r="AC57" s="26"/>
+      <c r="AD57" s="27"/>
+      <c r="AE57" s="25"/>
+      <c r="AF57" s="26"/>
+      <c r="AG57" s="27"/>
+      <c r="AH57" s="25"/>
+      <c r="AI57" s="26"/>
+      <c r="AJ57" s="27"/>
+      <c r="AK57" s="25"/>
+      <c r="AL57" s="26"/>
+      <c r="AM57" s="27"/>
     </row>
     <row r="58" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C58" s="81" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D58" s="25"/>
       <c r="E58" s="25"/>
@@ -4058,10 +4070,10 @@
     <row r="59" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A59" s="8"/>
       <c r="B59" s="29" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="C59" s="77" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D59" s="25"/>
       <c r="E59" s="25"/>
@@ -4105,10 +4117,10 @@
     <row r="60" spans="1:39" s="62" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="58" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C60" s="78" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D60" s="60"/>
       <c r="E60" s="60"/>
@@ -4150,7 +4162,7 @@
     <row r="61" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C61" s="79" t="s">
         <v>29</v>
@@ -4195,7 +4207,7 @@
     <row r="62" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
       <c r="B62" s="29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C62" s="76" t="s">
         <v>91</v>
@@ -4223,7 +4235,8 @@
       <c r="X62" s="27"/>
       <c r="Y62" s="25"/>
       <c r="Z62" s="26"/>
-      <c r="AA62" s="27"/>
+      <c r="AA62" s="105"/>
+      <c r="AB62" s="106"/>
       <c r="AC62" s="26"/>
       <c r="AD62" s="27"/>
       <c r="AE62" s="25">
@@ -4241,7 +4254,7 @@
     <row r="63" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
       <c r="B63" s="29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C63" s="76" t="s">
         <v>92</v>
@@ -4269,7 +4282,8 @@
       <c r="X63" s="27"/>
       <c r="Y63" s="25"/>
       <c r="Z63" s="26"/>
-      <c r="AA63" s="27"/>
+      <c r="AA63" s="105"/>
+      <c r="AB63" s="106"/>
       <c r="AC63" s="26"/>
       <c r="AD63" s="27"/>
       <c r="AE63" s="25">
@@ -4287,10 +4301,10 @@
     <row r="64" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
       <c r="B64" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C64" s="76" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D64" s="25"/>
       <c r="E64" s="25"/>
@@ -4315,7 +4329,8 @@
       <c r="X64" s="27"/>
       <c r="Y64" s="25"/>
       <c r="Z64" s="26"/>
-      <c r="AA64" s="27"/>
+      <c r="AA64" s="105"/>
+      <c r="AB64" s="106"/>
       <c r="AC64" s="26"/>
       <c r="AD64" s="27"/>
       <c r="AE64" s="25">
@@ -4333,10 +4348,10 @@
     <row r="65" spans="1:39" s="62" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
       <c r="B65" s="58" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C65" s="78" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D65" s="60"/>
       <c r="E65" s="60"/>
@@ -4378,10 +4393,10 @@
     <row r="66" spans="1:39" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="8"/>
       <c r="B66" s="57" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C66" s="82" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D66" s="65"/>
       <c r="E66" s="65"/>
@@ -4423,10 +4438,10 @@
     <row r="67" spans="1:39" s="71" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
       <c r="B67" s="63" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C67" s="76" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D67" s="69"/>
       <c r="E67" s="69"/>
@@ -4469,10 +4484,10 @@
     <row r="68" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="B68" s="63" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C68" s="76" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D68" s="25"/>
       <c r="E68" s="25"/>
@@ -4513,10 +4528,10 @@
     <row r="69" spans="1:39" s="62" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="58" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C69" s="78" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D69" s="60"/>
       <c r="E69" s="60"/>
@@ -4913,11 +4928,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="J10:L10"/>
     <mergeCell ref="AB10:AD10"/>
     <mergeCell ref="AE10:AG10"/>
     <mergeCell ref="AH10:AJ10"/>
@@ -4928,6 +4938,11 @@
     <mergeCell ref="S10:U10"/>
     <mergeCell ref="V10:X10"/>
     <mergeCell ref="Y10:AA10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="J10:L10"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -4936,15 +4951,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100CCA9B0B81E3CB9409C129017DE6E9DDD" ma:contentTypeVersion="13" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="b4d33a61f6d93acd2f5bb33bcd02c3da">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5377820a-2d68-4adb-aaae-bcf0ba6bf8f0" xmlns:ns4="5835faf6-6bc7-44cd-9638-9d00e184b482" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1e23a8e84f7c9cb6cabb5016b2cfc6c5" ns3:_="" ns4:_="">
     <xsd:import namespace="5377820a-2d68-4adb-aaae-bcf0ba6bf8f0"/>
@@ -5167,6 +5173,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -5174,14 +5189,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{662529E2-C398-4237-A004-9E9B5846A970}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEA18E47-C9B6-4A69-AAAC-F358C569EB24}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5196,6 +5203,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{662529E2-C398-4237-A004-9E9B5846A970}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>